<commit_message>
Fixed xlss update for BARs
</commit_message>
<xml_diff>
--- a/dramatis_personae.xlsx
+++ b/dramatis_personae.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Abstract" sheetId="1" state="visible" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <t>Release date</t>
   </si>
   <si>
-    <t>2018-06-23 21:24:59.584573</t>
+    <t>2018-07-06 15:59:55.744085</t>
   </si>
   <si>
     <t>Dramatis Personae</t>
@@ -2584,10 +2584,64 @@
     <t>Value</t>
   </si>
   <si>
+    <t>Addiction</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>-4</t>
+  </si>
+  <si>
+    <t>Alien Upbringing</t>
+  </si>
+  <si>
+    <t>Ally</t>
+  </si>
+  <si>
+    <t>Cloistered</t>
+  </si>
+  <si>
+    <t>ot</t>
+  </si>
+  <si>
+    <t>Dark Secret</t>
+  </si>
+  <si>
+    <t>Heir</t>
+  </si>
+  <si>
+    <t>Infamous Family</t>
+  </si>
+  <si>
+    <t>Lost Worlder</t>
+  </si>
+  <si>
+    <t>Oath of Fealty</t>
+  </si>
+  <si>
+    <t>Obligation</t>
+  </si>
+  <si>
+    <t>Orphan</t>
+  </si>
+  <si>
     <t>Secrets</t>
   </si>
   <si>
-    <t>ba</t>
+    <t>Stigma</t>
+  </si>
+  <si>
+    <t>Vow of Celibacy</t>
+  </si>
+  <si>
+    <t>Vow of Poverty</t>
+  </si>
+  <si>
+    <t>Vow of Silence</t>
   </si>
   <si>
     <t>Well-Traveled</t>
@@ -2596,61 +2650,7 @@
     <t>Known Worlds</t>
   </si>
   <si>
-    <t>Heir</t>
-  </si>
-  <si>
-    <t>ot</t>
-  </si>
-  <si>
     <t>Major house Fief</t>
-  </si>
-  <si>
-    <t>Alien Upbringing</t>
-  </si>
-  <si>
-    <t>Ally</t>
-  </si>
-  <si>
-    <t>Dark Secret</t>
-  </si>
-  <si>
-    <t>Infamous Family</t>
-  </si>
-  <si>
-    <t>Lost Worlder</t>
-  </si>
-  <si>
-    <t>Oath of Fealty</t>
-  </si>
-  <si>
-    <t>Obligation</t>
-  </si>
-  <si>
-    <t>Orphan</t>
-  </si>
-  <si>
-    <t>Stigma</t>
-  </si>
-  <si>
-    <t>Vow of Celibacy</t>
-  </si>
-  <si>
-    <t>Cloistered</t>
-  </si>
-  <si>
-    <t>Addiction</t>
-  </si>
-  <si>
-    <t>Vow of Poverty</t>
-  </si>
-  <si>
-    <t>-3</t>
-  </si>
-  <si>
-    <t>Vow of Silence</t>
-  </si>
-  <si>
-    <t>-4</t>
   </si>
 </sst>
 </file>
@@ -15829,25 +15829,27 @@
         <v>854</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>539</v>
       </c>
       <c r="C3" t="s">
         <v>855</v>
       </c>
-      <c r="D3" t="s"/>
+      <c r="D3" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>854</v>
+      </c>
+      <c r="B4" t="s">
         <v>856</v>
-      </c>
-      <c r="B4" t="s">
-        <v>44</v>
       </c>
       <c r="C4" t="s">
         <v>855</v>
       </c>
       <c r="D4" t="s">
-        <v>857</v>
+        <v>643</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -15855,102 +15857,116 @@
         <v>854</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>857</v>
       </c>
       <c r="C5" t="s">
         <v>855</v>
       </c>
-      <c r="D5" t="s"/>
+      <c r="D5" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>858</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
         <v>855</v>
       </c>
-      <c r="D6" t="s"/>
+      <c r="D6" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>854</v>
+        <v>859</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>553</v>
       </c>
       <c r="C7" t="s">
-        <v>855</v>
-      </c>
-      <c r="D7" t="s"/>
+        <v>670</v>
+      </c>
+      <c r="D7" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>580</v>
       </c>
       <c r="C8" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="D8" t="s">
-        <v>860</v>
+        <v>643</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>580</v>
       </c>
       <c r="C9" t="s">
         <v>855</v>
       </c>
-      <c r="D9" t="s"/>
+      <c r="D9" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>854</v>
+        <v>862</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>539</v>
       </c>
       <c r="C10" t="s">
         <v>855</v>
       </c>
-      <c r="D10" t="s"/>
+      <c r="D10" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>854</v>
+        <v>862</v>
       </c>
       <c r="B11" t="s">
-        <v>553</v>
+        <v>856</v>
       </c>
       <c r="C11" t="s">
         <v>855</v>
       </c>
-      <c r="D11" t="s"/>
+      <c r="D11" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B12" t="s">
-        <v>553</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>670</v>
-      </c>
-      <c r="D12" t="s"/>
+        <v>855</v>
+      </c>
+      <c r="D12" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="B13" t="s">
         <v>580</v>
@@ -15958,11 +15974,13 @@
       <c r="C13" t="s">
         <v>855</v>
       </c>
-      <c r="D13" t="s"/>
+      <c r="D13" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B14" t="s">
         <v>580</v>
@@ -15970,11 +15988,13 @@
       <c r="C14" t="s">
         <v>855</v>
       </c>
-      <c r="D14" t="s"/>
+      <c r="D14" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B15" t="s">
         <v>580</v>
@@ -15982,35 +16002,41 @@
       <c r="C15" t="s">
         <v>855</v>
       </c>
-      <c r="D15" t="s"/>
+      <c r="D15" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>866</v>
       </c>
       <c r="B16" t="s">
-        <v>580</v>
+        <v>539</v>
       </c>
       <c r="C16" t="s">
         <v>855</v>
       </c>
-      <c r="D16" t="s"/>
+      <c r="D16" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B17" t="s">
-        <v>580</v>
+        <v>856</v>
       </c>
       <c r="C17" t="s">
         <v>855</v>
       </c>
-      <c r="D17" t="s"/>
+      <c r="D17" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B18" t="s">
         <v>580</v>
@@ -16018,211 +16044,247 @@
       <c r="C18" t="s">
         <v>855</v>
       </c>
-      <c r="D18" t="s"/>
+      <c r="D18" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B19" t="s">
-        <v>580</v>
+        <v>539</v>
       </c>
       <c r="C19" t="s">
         <v>855</v>
       </c>
-      <c r="D19" t="s"/>
+      <c r="D19" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="B20" t="s">
-        <v>580</v>
+        <v>856</v>
       </c>
       <c r="C20" t="s">
         <v>855</v>
       </c>
-      <c r="D20" t="s"/>
+      <c r="D20" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="B21" t="s">
         <v>580</v>
       </c>
       <c r="C21" t="s">
-        <v>859</v>
-      </c>
-      <c r="D21" t="s"/>
+        <v>855</v>
+      </c>
+      <c r="D21" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B22" t="s">
-        <v>539</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
         <v>855</v>
       </c>
-      <c r="D22" t="s"/>
+      <c r="D22" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>863</v>
+        <v>869</v>
       </c>
       <c r="B23" t="s">
-        <v>539</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
         <v>855</v>
       </c>
-      <c r="D23" t="s"/>
+      <c r="D23" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>866</v>
+        <v>869</v>
       </c>
       <c r="B24" t="s">
-        <v>539</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
         <v>855</v>
       </c>
-      <c r="D24" t="s"/>
+      <c r="D24" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="B25" t="s">
-        <v>539</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
         <v>855</v>
       </c>
-      <c r="D25" t="s"/>
+      <c r="D25" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>869</v>
       </c>
       <c r="B26" t="s">
-        <v>539</v>
+        <v>553</v>
       </c>
       <c r="C26" t="s">
         <v>855</v>
       </c>
-      <c r="D26" t="s"/>
+      <c r="D26" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="B27" t="s">
-        <v>539</v>
+        <v>580</v>
       </c>
       <c r="C27" t="s">
         <v>855</v>
       </c>
-      <c r="D27" t="s"/>
+      <c r="D27" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="B28" t="s">
-        <v>874</v>
+        <v>539</v>
       </c>
       <c r="C28" t="s">
         <v>855</v>
       </c>
-      <c r="D28" t="s"/>
+      <c r="D28" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>863</v>
+        <v>870</v>
       </c>
       <c r="B29" t="s">
-        <v>874</v>
+        <v>856</v>
       </c>
       <c r="C29" t="s">
         <v>855</v>
       </c>
-      <c r="D29" t="s"/>
+      <c r="D29" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="B30" t="s">
-        <v>874</v>
+        <v>857</v>
       </c>
       <c r="C30" t="s">
         <v>855</v>
       </c>
-      <c r="D30" t="s"/>
+      <c r="D30" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>867</v>
+        <v>871</v>
       </c>
       <c r="B31" t="s">
-        <v>874</v>
+        <v>580</v>
       </c>
       <c r="C31" t="s">
         <v>855</v>
       </c>
-      <c r="D31" t="s"/>
+      <c r="D31" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>869</v>
+        <v>872</v>
       </c>
       <c r="B32" t="s">
-        <v>874</v>
+        <v>539</v>
       </c>
       <c r="C32" t="s">
         <v>855</v>
       </c>
-      <c r="D32" t="s"/>
+      <c r="D32" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B33" t="s">
-        <v>874</v>
+        <v>856</v>
       </c>
       <c r="C33" t="s">
         <v>855</v>
       </c>
-      <c r="D33" t="s"/>
+      <c r="D33" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="B34" t="s">
-        <v>876</v>
+        <v>44</v>
       </c>
       <c r="C34" t="s">
         <v>855</v>
       </c>
-      <c r="D34" t="s"/>
+      <c r="D34" t="s">
+        <v>875</v>
+      </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>869</v>
+        <v>874</v>
       </c>
       <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
+        <v>861</v>
+      </c>
+      <c r="D35" t="s">
         <v>876</v>
       </c>
-      <c r="C35" t="s">
-        <v>855</v>
-      </c>
-      <c r="D35" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>